<commit_message>
Added contribution to public group
</commit_message>
<xml_diff>
--- a/InterviewQuestions/Q_A-Azure.xlsx
+++ b/InterviewQuestions/Q_A-Azure.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deevita Pharmacy TM\Downloads\azurelearning\AzureLearning\InterviewQuestions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deevita Pharmacy TM\Downloads\azurestuffs\AzureStuffs\InterviewQuestions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4C0B20-76DC-4FBC-BD63-22DD4DD1D125}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF20FDA-F92C-4D3C-8088-F54ECB71B3DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{42744AD4-9A8B-4D33-B2E6-4F91E852CE0A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{42744AD4-9A8B-4D33-B2E6-4F91E852CE0A}"/>
   </bookViews>
   <sheets>
     <sheet name="ADF" sheetId="1" r:id="rId1"/>
     <sheet name="Azure DATABRICKS" sheetId="2" r:id="rId2"/>
+    <sheet name="General" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
   <si>
     <t>Question</t>
   </si>
@@ -2151,12 +2152,52 @@
       <t xml:space="preserve"> "notebook-path"</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">via web browser, link is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>portal.azure.com</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>How you access</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> azure portal and link?</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2166,6 +2207,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -2713,8 +2763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6F94638-29F7-4A2B-B9B2-AA971557FEE3}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2893,4 +2943,47 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D3891C4-D980-44C0-948A-018E4D5CDB38}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>